<commit_message>
fixed bugs #1 - #4
</commit_message>
<xml_diff>
--- a/Triangles/debuggingFixRecord.xlsx
+++ b/Triangles/debuggingFixRecord.xlsx
@@ -15,7 +15,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Test Suite</t>
   </si>
@@ -91,6 +90,21 @@
   </si>
   <si>
     <t>#3 changed an 'X" to a "Y" in Edge.cpp line 21</t>
+  </si>
+  <si>
+    <t>EdgeTester::testEdge01</t>
+  </si>
+  <si>
+    <t>testing e.getSlopeZ</t>
+  </si>
+  <si>
+    <t>not setting value to inf</t>
+  </si>
+  <si>
+    <t>#4</t>
+  </si>
+  <si>
+    <t>#4 changed "!=" to "==" Edge.cpp line 94</t>
   </si>
 </sst>
 </file>
@@ -478,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E24"/>
+  <dimension ref="B1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -548,10 +562,18 @@
       </c>
     </row>
     <row r="6" spans="2:5" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
+      <c r="B6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="7" spans="2:5" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
@@ -639,6 +661,11 @@
         <v>21</v>
       </c>
     </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B26" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
bug fixes through #7 added
</commit_message>
<xml_diff>
--- a/Triangles/debuggingFixRecord.xlsx
+++ b/Triangles/debuggingFixRecord.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="47">
   <si>
     <t>Test Suite</t>
   </si>
@@ -105,6 +105,66 @@
   </si>
   <si>
     <t>#4 changed "!=" to "==" Edge.cpp line 94</t>
+  </si>
+  <si>
+    <t>testFirstConstructor</t>
+  </si>
+  <si>
+    <t>t.getTriangleType()!='S'</t>
+  </si>
+  <si>
+    <t>Expected 'S' but returned 'N'</t>
+  </si>
+  <si>
+    <t>#5</t>
+  </si>
+  <si>
+    <t>if (isTriangle())</t>
+  </si>
+  <si>
+    <t>if (!isTriangle())</t>
+  </si>
+  <si>
+    <t>CHAGNED TO</t>
+  </si>
+  <si>
+    <t>#5 Triangle.cpp line 64</t>
+  </si>
+  <si>
+    <t>Expected 'S' but returned 'I'</t>
+  </si>
+  <si>
+    <t>#6</t>
+  </si>
+  <si>
+    <t>#6 Triangle.cpp line 76</t>
+  </si>
+  <si>
+    <t>appromixatelyEquals(c,a,m_edgeLengthThreshold))</t>
+  </si>
+  <si>
+    <t>appromixatelyEquals(c,c,m_edgeLengthThreshold))</t>
+  </si>
+  <si>
+    <t>CHANGED TO</t>
+  </si>
+  <si>
+    <t>#7 Triangle.cpp line 105</t>
+  </si>
+  <si>
+    <t>Test compute area</t>
+  </si>
+  <si>
+    <t>Giving unexpected area</t>
+  </si>
+  <si>
+    <t>#7</t>
+  </si>
+  <si>
+    <t>double s = ( a + b + c)/2;</t>
+  </si>
+  <si>
+    <t>double s = ( a + b + b)/2;</t>
   </si>
 </sst>
 </file>
@@ -492,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E26"/>
+  <dimension ref="B1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -576,22 +636,42 @@
       </c>
     </row>
     <row r="7" spans="2:5" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="8" spans="2:5" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+      <c r="C8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="9" spans="2:5" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+      <c r="C9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="10" spans="2:5" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
@@ -666,6 +746,54 @@
         <v>26</v>
       </c>
     </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B29" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B31" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B32" t="s">
+        <v>40</v>
+      </c>
+      <c r="C32" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B34" t="s">
+        <v>41</v>
+      </c>
+      <c r="C34" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B35" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>